<commit_message>
minor changes in folder name
</commit_message>
<xml_diff>
--- a/source/samples/export/iTinExportEngineSamples/output/xlsx/EPPlus/sample06-from-config-file.xlsx
+++ b/source/samples/export/iTinExportEngineSamples/output/xlsx/EPPlus/sample06-from-config-file.xlsx
@@ -1064,7 +1064,7 @@
   <extLst>
     <ext uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{0c3c2d58-55f5-4be8-8963-2f400b98717e}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8c6e192f-301b-43b2-a6ff-364086c51090}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1080,7 +1080,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4caa0bbb-73e5-45b6-af76-d0e44031c237}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{76f1f6e4-7aff-4a9e-8872-85ee487f57e6}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1096,7 +1096,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a60eb108-c691-461b-917f-15aaf87ac1db}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{38059eec-d111-4ad8-99be-921da9287871}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1112,7 +1112,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{174221d9-cbc3-4e36-9ac2-447856a21989}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{56dcb7ee-787f-4ad8-b6fd-e0a3acda6cd0}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1128,7 +1128,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c87b5f97-855e-4614-b412-0438fa3738e8}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{7cab3c98-f256-4dd2-8578-d57e068fd468}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1144,7 +1144,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d2ea5d2f-40cf-4e88-bf6d-781d4cda9cce}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c0127a9d-7b89-4bbb-933d-8870d67ab195}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1160,7 +1160,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a993edb9-65b6-4004-9250-b1866d1b9a51}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{3d9ae965-8639-4305-b084-ca9c51982775}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1176,7 +1176,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b8f21908-c2bc-414a-a1d1-3ef2ae28c5c4}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b8a20692-0aa4-46e4-93fb-8c1ba967b861}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1192,7 +1192,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{fec70475-6950-41df-8eb0-186f75dcdb52}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{3f3cf8fe-c774-40de-8b51-664c3cb8090b}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1208,7 +1208,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{cd2e669c-ed6d-4b3e-bf7d-44bad94c30d3}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{01299688-13ec-4db5-8eda-b17476c00804}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1224,7 +1224,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{772a5ada-0cc3-4bc5-acbf-66a70700db17}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8605975f-1eb2-457c-b595-fd28493894d9}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1240,7 +1240,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{005285e1-b772-4a40-8c4a-1b33392c4735}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{53605129-54c9-4d6e-8d52-4c0786cfed89}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1256,7 +1256,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e6f75b48-ed9e-4960-89d6-917cceaad5fd}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{5a85a148-0f84-4d85-a367-8d1f6b4370a7}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1272,7 +1272,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2e84de4f-19ad-49a3-933b-8746b080e68c}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b665bf5d-f881-4019-9df0-3d6c713d497e}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1288,7 +1288,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{10bc3551-06eb-4822-a708-1d400eb74217}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8805538d-da08-41db-bf46-eda6bb315ea9}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1304,7 +1304,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{12e7220f-0625-44a3-9c2b-e1660dfe4ebf}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{566101a4-8a14-44e1-8b79-dc79d5f6b158}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1320,7 +1320,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{cd76ec46-6e36-4209-b696-6c51385b2de6}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b68e85f3-d5f7-444b-b8f1-9d4beb068044}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1338,7 +1338,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{00f98480-a6f3-48f4-9a47-d89f6d082081}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a12ac9e2-d547-4966-afca-d1b1a8e1d2d4}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1356,7 +1356,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d448156e-f9aa-442e-9ec1-5659dd12a3a4}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{11bff325-7d19-4369-8325-a3811cdc49b9}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1374,7 +1374,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f628c764-8e8c-4cd0-b964-6fdb38255b96}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4c811377-6e3d-4cca-9bf0-af8c1c1bd8ae}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1392,7 +1392,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{86f69beb-8dfb-40a5-a6a7-bfc66d13582f}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{3db9ba09-82b4-4aea-8cea-f412dc715a03}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1410,7 +1410,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{5913fe72-2957-4e25-86c1-ca43e3983670}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b9f10b8d-5f87-4d26-a881-3eb2ed1629db}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1428,7 +1428,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f30cbc7c-85ae-4f94-8fb8-90d30f05d987}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{bdaeecc5-86fc-4dd0-bd29-f272ed2b9d10}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1446,7 +1446,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{03f06d1c-3197-413c-89f3-0ca78fe304b2}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{fc2ffc65-4b16-4b18-b0a1-d64e6dca5515}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1464,7 +1464,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{37c808ae-e9cf-4248-9225-1ebf21c336e0}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b7afe9ad-ca8c-4aac-87c8-9b1010b05e5d}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1482,7 +1482,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4e8d13c8-61d8-4706-a8a8-5ed7e12ab55a}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{63bd67a6-29ab-40f9-924b-37e354eed207}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1500,7 +1500,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d2e30ec2-0263-44fd-8b29-5acedd5f4667}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f958518c-b616-4b99-bc78-24447648d718}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1518,7 +1518,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{511aa3e1-4deb-44d0-807f-40f88ff799bf}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{fd576655-16f7-42f3-9011-284970f59d83}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1536,7 +1536,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a485be31-7ef2-46c8-b059-9117f19446da}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{da98326a-2992-4a94-80b4-b7a37f40361f}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1554,7 +1554,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f2fd8874-8a59-4a27-90f7-3c33ecf01f13}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f04a080b-2fec-4819-bf97-371629a01021}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1572,7 +1572,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{9dea1fed-5167-490e-bac6-8cdff72b349d}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f35de518-348f-43d1-89d9-cdb8f50b31d6}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1590,7 +1590,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e174b64b-bba9-4d3c-a666-fc6cabde9ac9}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a8d9862d-8199-47ed-9e1a-cfe0ae68ce1b}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>

</xml_diff>

<commit_message>
Adds transform behavior configuration to xml export configuration
</commit_message>
<xml_diff>
--- a/source/samples/export/iTinExportEngineSamples/output/xlsx/EPPlus/sample06-from-config-file.xlsx
+++ b/source/samples/export/iTinExportEngineSamples/output/xlsx/EPPlus/sample06-from-config-file.xlsx
@@ -1064,7 +1064,7 @@
   <extLst>
     <ext uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8c6e192f-301b-43b2-a6ff-364086c51090}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8ccc79d0-3ee6-4f87-a6ec-4182198c13b4}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1080,7 +1080,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{76f1f6e4-7aff-4a9e-8872-85ee487f57e6}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{aaaeb641-a7da-48aa-ba2c-1dc82f66b256}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1096,7 +1096,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{38059eec-d111-4ad8-99be-921da9287871}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{faa53d77-eda1-4cc0-81c8-7394f589469c}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1112,7 +1112,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{56dcb7ee-787f-4ad8-b6fd-e0a3acda6cd0}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a7f2ee5e-df0a-4f25-9240-d8d76212f693}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1128,7 +1128,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{7cab3c98-f256-4dd2-8578-d57e068fd468}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{86df9801-e633-4296-9269-c3f4c1037e28}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1144,7 +1144,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c0127a9d-7b89-4bbb-933d-8870d67ab195}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{27f1a813-d556-4ed8-989c-c6fdbbaa4c30}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1160,7 +1160,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{3d9ae965-8639-4305-b084-ca9c51982775}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{1568803f-2e11-4054-8894-e7272d3f2c4a}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1176,7 +1176,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b8a20692-0aa4-46e4-93fb-8c1ba967b861}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a7f53258-8aa5-4aa0-b3d9-e887bb8ea6e2}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1192,7 +1192,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{3f3cf8fe-c774-40de-8b51-664c3cb8090b}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{60f50964-172b-4e6e-b7a9-479bc505b704}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1208,7 +1208,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{01299688-13ec-4db5-8eda-b17476c00804}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8935b24d-f612-460c-aac6-04cd6f21965a}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1224,7 +1224,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8605975f-1eb2-457c-b595-fd28493894d9}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{312c8dd1-3052-49e3-8243-28b6c61e64aa}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1240,7 +1240,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{53605129-54c9-4d6e-8d52-4c0786cfed89}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2a544b44-8864-4baa-8834-bd3451389136}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1256,7 +1256,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{5a85a148-0f84-4d85-a367-8d1f6b4370a7}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b1c04135-4779-46dd-b6da-eaf5830cf9f1}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1272,7 +1272,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b665bf5d-f881-4019-9df0-3d6c713d497e}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f7d6d4e5-0005-43b0-a1a3-83733ea0f0fc}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1288,7 +1288,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8805538d-da08-41db-bf46-eda6bb315ea9}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{37165d0e-ae5d-4e37-9f75-24dc845f73d9}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1304,7 +1304,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{566101a4-8a14-44e1-8b79-dc79d5f6b158}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{81567066-713a-4c30-bd66-7837cb5de376}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1320,7 +1320,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b68e85f3-d5f7-444b-b8f1-9d4beb068044}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{bafdba06-751b-4c30-aa2e-430026d749d7}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1338,7 +1338,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a12ac9e2-d547-4966-afca-d1b1a8e1d2d4}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4e0d3f53-0317-440b-9d1b-3f900e64002a}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1356,7 +1356,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{11bff325-7d19-4369-8325-a3811cdc49b9}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{7ee1f089-deed-47f1-9679-703ecc335458}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1374,7 +1374,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4c811377-6e3d-4cca-9bf0-af8c1c1bd8ae}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{02394c75-4ee7-4157-8966-406936522aca}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1392,7 +1392,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{3db9ba09-82b4-4aea-8cea-f412dc715a03}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8197057c-7a03-4a26-aa77-33d3b5a9a334}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1410,7 +1410,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b9f10b8d-5f87-4d26-a881-3eb2ed1629db}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d2dcfd73-a484-40b7-b261-d746e788cadc}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1428,7 +1428,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{bdaeecc5-86fc-4dd0-bd29-f272ed2b9d10}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f5e866b5-9831-4f2b-9411-b2302a941a68}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1446,7 +1446,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{fc2ffc65-4b16-4b18-b0a1-d64e6dca5515}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{bf854a6a-92aa-4b9d-b6bd-ad301d0b950c}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1464,7 +1464,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b7afe9ad-ca8c-4aac-87c8-9b1010b05e5d}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{6247b22c-e9e0-40ed-be8f-69492420944b}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1482,7 +1482,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{63bd67a6-29ab-40f9-924b-37e354eed207}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4faeb6de-e984-4869-9344-7bb139ad2928}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1500,7 +1500,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f958518c-b616-4b99-bc78-24447648d718}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{7ebdda71-ae5b-43ae-b139-0e40af2220fd}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1518,7 +1518,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{fd576655-16f7-42f3-9011-284970f59d83}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e51feb26-0255-4e8e-8126-dcbd660ee915}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1536,7 +1536,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{da98326a-2992-4a94-80b4-b7a37f40361f}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{16d885d9-7b05-4c05-ae74-05d22bc6dd89}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1554,7 +1554,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f04a080b-2fec-4819-bf97-371629a01021}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b7d6e073-9acc-4958-a45c-9bc5dd81cadc}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1572,7 +1572,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f35de518-348f-43d1-89d9-cdb8f50b31d6}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{aecfab4f-deb5-4b1d-9995-d2496cdd4995}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1590,7 +1590,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a8d9862d-8199-47ed-9e1a-cfe0ae68ce1b}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e5e2649b-b47d-46b7-99b4-76c9adf8a869}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>

</xml_diff>

<commit_message>
Add Create attribute in Table>Output element
</commit_message>
<xml_diff>
--- a/source/samples/export/iTinExportEngineSamples/output/xlsx/EPPlus/sample06-from-config-file.xlsx
+++ b/source/samples/export/iTinExportEngineSamples/output/xlsx/EPPlus/sample06-from-config-file.xlsx
@@ -1064,7 +1064,7 @@
   <extLst>
     <ext uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8ccc79d0-3ee6-4f87-a6ec-4182198c13b4}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{6fa03570-9b14-4bf5-a56d-b391e88b22f0}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1080,7 +1080,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{aaaeb641-a7da-48aa-ba2c-1dc82f66b256}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{afa27860-3a49-44ca-bd88-3d5679b62fc9}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1096,7 +1096,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{faa53d77-eda1-4cc0-81c8-7394f589469c}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{955537b9-d9a3-45d0-aa0b-1d6ca2064aff}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1112,7 +1112,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a7f2ee5e-df0a-4f25-9240-d8d76212f693}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{7934398e-7f45-437b-84ce-dff360ba45be}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1128,7 +1128,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{86df9801-e633-4296-9269-c3f4c1037e28}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{620e46ed-ff56-4830-8366-58eedea456a0}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1144,7 +1144,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{27f1a813-d556-4ed8-989c-c6fdbbaa4c30}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2d002ba6-76ce-44ff-9c7b-4940fb364e4e}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1160,7 +1160,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{1568803f-2e11-4054-8894-e7272d3f2c4a}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d4bf6ee8-d0d8-45be-9961-7dfc6b8698ff}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1176,7 +1176,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a7f53258-8aa5-4aa0-b3d9-e887bb8ea6e2}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d9ad0962-4033-49c9-a696-ed050b408d1f}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1192,7 +1192,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{60f50964-172b-4e6e-b7a9-479bc505b704}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{97604903-a1eb-47fc-aa58-0f6730485a0c}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1208,7 +1208,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8935b24d-f612-460c-aac6-04cd6f21965a}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{5dd6dc89-5b7c-40c5-a7b0-448ef9f36acb}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1224,7 +1224,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{312c8dd1-3052-49e3-8243-28b6c61e64aa}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{3e17084a-b5c8-4170-8bb0-14973bcfd3b2}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1240,7 +1240,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2a544b44-8864-4baa-8834-bd3451389136}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e0e5ee90-cf08-4f5d-b878-befe0e8f0753}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1256,7 +1256,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b1c04135-4779-46dd-b6da-eaf5830cf9f1}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b9df0b18-9044-489e-bc65-74e043a76963}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1272,7 +1272,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f7d6d4e5-0005-43b0-a1a3-83733ea0f0fc}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{cfbeb4cd-5bc8-4b4e-b179-0996c91c7927}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1288,7 +1288,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{37165d0e-ae5d-4e37-9f75-24dc845f73d9}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{fa1f1c79-b58c-45f2-8f24-5bcd6da9f551}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1304,7 +1304,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{81567066-713a-4c30-bd66-7837cb5de376}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{6905faa0-493d-4bd5-a432-8265aeee4aee}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1320,7 +1320,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{bafdba06-751b-4c30-aa2e-430026d749d7}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{3fc80200-4f76-4dab-974d-5713677ca91b}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1338,7 +1338,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4e0d3f53-0317-440b-9d1b-3f900e64002a}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a2af62d0-434c-4c02-b3db-36797610805e}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1356,7 +1356,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{7ee1f089-deed-47f1-9679-703ecc335458}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{23fe3aa2-e2b7-4270-a81e-34798a8692bb}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1374,7 +1374,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{02394c75-4ee7-4157-8966-406936522aca}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{3de5ff35-36de-4fcb-b093-32632da9366c}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1392,7 +1392,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8197057c-7a03-4a26-aa77-33d3b5a9a334}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e73daa8f-5b56-4b42-b5b7-226f669b50bc}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1410,7 +1410,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d2dcfd73-a484-40b7-b261-d746e788cadc}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{bf49d508-7e34-474a-beea-5a06b4705990}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1428,7 +1428,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f5e866b5-9831-4f2b-9411-b2302a941a68}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c45b8001-f2c3-417b-9031-71fcb4e9ffd3}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1446,7 +1446,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{bf854a6a-92aa-4b9d-b6bd-ad301d0b950c}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{952884d4-28e2-47d3-b421-ca3fa592ff0b}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1464,7 +1464,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{6247b22c-e9e0-40ed-be8f-69492420944b}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{10a78a16-ad19-4e87-b78d-86575e0079da}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1482,7 +1482,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4faeb6de-e984-4869-9344-7bb139ad2928}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2481a3b6-063a-4758-805a-3a03cc22c47c}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1500,7 +1500,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{7ebdda71-ae5b-43ae-b139-0e40af2220fd}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f78d8c46-bf27-49d8-b485-2ca68ace839d}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1518,7 +1518,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e51feb26-0255-4e8e-8126-dcbd660ee915}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{fa63ac39-8fc1-4c9c-b04c-6db08d187cf7}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1536,7 +1536,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{16d885d9-7b05-4c05-ae74-05d22bc6dd89}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f9ce5678-ae29-46fc-8b39-25027b1832c2}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1554,7 +1554,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b7d6e073-9acc-4958-a45c-9bc5dd81cadc}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{69552712-a2fe-4408-ac18-390a37b85a4f}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1572,7 +1572,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{aecfab4f-deb5-4b1d-9995-d2496cdd4995}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{fb4fae7c-da54-4047-98bc-852519514e53}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1590,7 +1590,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e5e2649b-b47d-46b7-99b4-76c9adf8a869}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{39d517eb-0a8c-4e61-a622-478d020c4d18}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>

</xml_diff>

<commit_message>
Add constructor to BaseDataField class
</commit_message>
<xml_diff>
--- a/source/samples/export/iTinExportEngineSamples/output/xlsx/EPPlus/sample06-from-config-file.xlsx
+++ b/source/samples/export/iTinExportEngineSamples/output/xlsx/EPPlus/sample06-from-config-file.xlsx
@@ -1064,7 +1064,7 @@
   <extLst>
     <ext uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f9beab1b-5810-47f6-b8de-d1d869dc2ebf}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b763aef2-d016-41fa-81f5-7f2b383dbe14}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1080,7 +1080,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b4cbe972-f660-4cff-ab6f-10a5d5484b39}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{761f241c-0dfb-43da-9a9f-4b926ade891d}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1096,7 +1096,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{cd61062e-9b00-4e20-bd4e-cc50352de191}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{3d0a7d05-c48a-42f2-8afa-85c6d9b99ccf}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1112,7 +1112,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{ac90d141-b826-4f48-835a-627d43bea72f}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{66e5f207-34c5-43ba-b823-d2ac915c1612}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1128,7 +1128,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e68a3b44-8c37-4383-9220-2cf03b1f5a7f}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a4cb3bfe-340c-4ef3-ba49-0bdaa4ba679c}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1144,7 +1144,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a850301d-a287-475c-ae7a-1d3923f629de}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2489d9c3-828f-4f0d-83f9-d1e26e43d49f}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1160,7 +1160,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2bf73a89-d92f-4ce7-a745-936c72fa61be}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f6792e82-4f61-40bf-aa61-fc9edee1cea5}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1176,7 +1176,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{48278435-aa2c-4176-956b-8e06478f06fc}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{1f8158a2-9280-42c5-8f77-a0fa4bbe478a}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1192,7 +1192,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{96c0bfcb-6f32-4157-a203-101a308a29f6}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{11a31e79-2db1-43b2-9dbe-1147967e498d}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1208,7 +1208,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{ad9c4bcf-8559-458e-aa12-040f4c50dced}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{ae6d9809-e1fe-4570-8608-6723585e6bed}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1224,7 +1224,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{0c26e275-79e1-433d-a088-6616461b988f}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{6f2fe23b-042a-470d-b05a-9fde1d828e1e}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1240,7 +1240,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{be473c78-d0c1-496a-8976-3a035b992fff}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{5e5e4629-cf42-4a89-b04f-7d2a5307a4dc}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1256,7 +1256,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{3ce500c2-5bfa-4251-ba0d-1265753334a7}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{9485f427-829d-4967-82bc-b636bf80fdc8}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1272,7 +1272,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8c9dfe76-3f54-40aa-b6bd-8f0872a041cf}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d59e1e53-ab7c-4349-a8ad-90c60632b5b9}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1288,7 +1288,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{7e36c4fd-69fa-40ed-9780-c0b524262aad}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{933706e0-6cd6-4531-959e-3e5abd965f1f}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1304,7 +1304,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4a53195b-bc6c-4faf-95ef-58268ffa9846}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{48afe6ff-2747-407c-af71-0621e3b4e19b}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1320,7 +1320,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{551d0c93-151e-4b29-bf7e-0c091086658f}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{6ac21f62-291e-406f-8bf4-666df643423a}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1338,7 +1338,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{60ad4c07-7fa8-40c9-a1ef-bd491bf08fa9}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{157191bf-755b-409e-a28c-cc2f576d13ff}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1356,7 +1356,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{21106c58-b289-496b-9654-81fcf4aa9823}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4dec0f4d-b494-4bc2-84ab-96bd1a6bade3}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1374,7 +1374,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b5ca71c6-fc5e-4958-8916-42f563139a04}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{6f303a92-1cd0-4cc6-83ea-af6b0d587a02}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1392,7 +1392,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{90442d8c-9ade-4043-9f45-b24e7ae06311}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{1447dd72-0a4b-4a67-9635-b2aeb32efa33}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1410,7 +1410,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{deed2cf2-13ac-4430-8211-b6258103d300}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b942afc7-9927-4134-b300-f20ea7fb3305}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1428,7 +1428,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{91762047-abff-40ce-83f2-6ed7f7eafb16}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{05c6b9aa-b513-46d0-a0d2-fa35fc61bbc1}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1446,7 +1446,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d2b4f404-2f28-41c3-9b6f-fdd77d924ba0}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e1c2f35e-dc10-4e66-9c30-086e7afd2a63}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1464,7 +1464,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d38a1a43-8bba-4cf8-817e-687ef9c0339f}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{bc2cabe1-1e3c-45eb-96b9-254d28ff77ca}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1482,7 +1482,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c91999d1-b2db-4754-be4b-660085a53c17}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f65bacae-7272-488e-a48a-4f81f7b95b61}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1500,7 +1500,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e396faa1-b9c6-4a7c-96d4-95495f32dd41}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{7f97c9fe-0260-4813-b538-66f204b38604}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1518,7 +1518,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8521de51-2b61-42a5-9cf7-b35565d571f4}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{856384c4-4db3-4f2c-8711-a11efb83a3d4}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1536,7 +1536,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{54e816dc-4986-4ecf-8b80-a964fb9f0dc8}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{eecb6f66-ba59-4841-8b09-9c497e99a716}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1554,7 +1554,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d39ead70-c754-4187-8d98-320ddfc1ac57}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{5f894d23-e05a-489f-8651-e9a78aed8931}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1572,7 +1572,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{125d4314-a5fa-4b5e-8093-91f9977d2391}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{63a9b33b-b722-4399-87ee-69480b098b82}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1590,7 +1590,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d46579c6-a41e-469c-ad9b-80e84a420264}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c4a8273d-5fa7-4609-96f9-382ccf43fa30}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>

</xml_diff>

<commit_message>
Add two new samples
</commit_message>
<xml_diff>
--- a/source/samples/export/iTinExportEngineSamples/output/xlsx/EPPlus/sample06-from-config-file.xlsx
+++ b/source/samples/export/iTinExportEngineSamples/output/xlsx/EPPlus/sample06-from-config-file.xlsx
@@ -1064,7 +1064,7 @@
   <extLst>
     <ext uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b60cbaa5-01ca-4f64-9c8a-e21d8c552921}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{7f601e94-6b88-4bc5-8678-f7af6a7289a6}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1080,7 +1080,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8dea60c7-4654-42aa-81e4-9aa2f402ce6a}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{fe9588fc-5fbd-4daa-8e60-d808efeeef92}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1096,7 +1096,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{7ee2e64e-b5bf-4cd2-8ffa-e87415c9c83d}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a779c4a9-7a23-4ae0-9188-af6de5f9fd44}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1112,7 +1112,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c67f6b46-ef37-4ba7-89a0-92750782c8b9}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{91e44f63-952c-4198-a909-7e1f9ea7880d}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1128,7 +1128,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{874dd29b-b9bb-4ae0-8ae0-978c1fdaf4f7}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{397b421d-0dd2-470c-88b8-f27f976ab327}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1144,7 +1144,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{46c6adeb-0cb5-405d-af50-c84ae376e00b}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4348135c-e831-4d7e-9f63-b595c8ca2a21}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1160,7 +1160,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{6052cb22-8e63-4292-a1a7-7d3e54e0dd66}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a018f1e1-2581-4132-9edf-2aeb96f4f9c5}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1176,7 +1176,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b1fa9035-4f00-4d55-ab7e-65dffc229c43}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{23e65482-2529-4c63-b813-fa71e94aa499}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1192,7 +1192,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a54f7302-2691-4767-8987-68fb28f41e19}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{5410fc0d-2d2a-4667-833f-79053e936acb}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1208,7 +1208,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c2111363-9b8f-46d2-b482-09a20f6bda68}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{1caaddde-9f8b-456a-a36e-c30995198589}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1224,7 +1224,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{ec2efee4-2de2-46ee-9294-06dab4a852fe}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{29bb8ebf-288a-4dc7-9d6a-5885b8779050}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1240,7 +1240,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{5865a727-0f1b-44a7-ad27-4d3dc802e5a6}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{bc37be61-3cf8-4b96-bd46-8b601da43e37}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1256,7 +1256,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c90b8303-63cc-4a1e-a438-bd2cadd824ab}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{6507d8e1-7579-4ee3-a85e-b4c09a6ac252}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1272,7 +1272,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a0e8d247-9c65-4233-b87d-9e5c8cf2f15b}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{103ac06c-b4fe-414e-a9e5-675122b8ca2e}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1288,7 +1288,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a7c142cf-297b-4a15-9f3d-90295ba148bc}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{cd1a2d2e-a65f-4508-8398-9ffa92cf8105}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1304,7 +1304,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f9d9107b-3e71-4966-8815-2576de60f585}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2504a5e7-31fd-494b-bba6-e7137e31a0d6}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1320,7 +1320,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{1d73420a-9e92-4a67-b344-d3b118a45f9a}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8199526c-e1e7-43f7-95bb-f6318d400fa2}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1338,7 +1338,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2349e6f1-52dc-4fab-97f7-5af904b6c237}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{66278097-82e0-4f14-981f-6179190897f6}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1356,7 +1356,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{6134b6bf-12b8-4eb5-b9cf-3fc3ea6f8789}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{0d8957bd-4de2-471b-8cf0-ad951fcddf60}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1374,7 +1374,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{64e0a9d9-ff72-47b0-8b9b-28765287f43f}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a50259dc-ea4b-4eb0-b07f-02233aa8e98b}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1392,7 +1392,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{e80976af-96ad-43d0-9f29-e51027fab8d8}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c00865e0-3331-4904-9dd6-84426eabb197}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1410,7 +1410,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{de109391-a2db-406d-b551-17654d1ffc91}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{7eebec89-9c7e-41ca-901e-8a32483f8c54}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1428,7 +1428,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{62c0e294-7549-4dcf-abaf-71622bdaa789}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a3a3d363-f78b-4d07-b7cc-b8e47078eea3}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1446,7 +1446,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{391aa4a6-d9a4-4f10-9584-829360210f9f}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{82ddfe5e-6d7a-490c-8b43-8cdf9f370ad2}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1464,7 +1464,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{3f5efadc-0b03-4722-9319-a01144c8ec4f}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{3f2afb21-89d1-429c-b54e-d0b607366a54}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1482,7 +1482,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8876dd5c-973b-4360-8e77-2ea9b294b1e2}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8ffa572d-59eb-4bc9-8277-47bcacb5257f}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1500,7 +1500,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{038272b9-f319-4f0d-8ad8-5c988a23a53c}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8cef9304-0307-43f6-a2b5-8855b7bd2c2e}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1518,7 +1518,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{cbb40420-7381-419d-aee8-6cf53c690bcc}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{512e5744-575b-4fab-bdd4-7225a65facd1}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1536,7 +1536,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{97748c80-02a9-4b9d-b2af-e65643988bf2}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4b3e4830-7432-4e5e-b92b-afa6492c26d8}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1554,7 +1554,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{0e737651-c987-418a-9d36-be2fea757290}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{6ae63daf-474b-4fd8-95ba-a2b1f9f25b44}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1572,7 +1572,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{3c335cb2-3376-43d8-8595-284e424be251}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f936dc8c-560a-46e7-b392-07597302fda9}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1590,7 +1590,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{02887acb-f3be-4159-b7b0-aa128692a68d}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2dfcc5cc-f843-4be7-93bc-4dd93b13868d}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>

</xml_diff>

<commit_message>
Markdown writer updated (support ShowDataValues attributte, font styles in header and values)
</commit_message>
<xml_diff>
--- a/source/samples/export/iTinExportEngineSamples/output/xlsx/EPPlus/sample06-from-config-file.xlsx
+++ b/source/samples/export/iTinExportEngineSamples/output/xlsx/EPPlus/sample06-from-config-file.xlsx
@@ -1064,7 +1064,7 @@
   <extLst>
     <ext uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{7f601e94-6b88-4bc5-8678-f7af6a7289a6}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a61b379d-db35-4b50-9d30-a2d8313851d7}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1080,7 +1080,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{fe9588fc-5fbd-4daa-8e60-d808efeeef92}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{80572990-7927-4009-b30c-7fb02fadc819}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1096,7 +1096,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a779c4a9-7a23-4ae0-9188-af6de5f9fd44}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4bb74453-8eaf-47a1-8c66-02deab9e582b}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1112,7 +1112,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{91e44f63-952c-4198-a909-7e1f9ea7880d}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{ee6ab2f0-59d5-4720-a870-9ca589103881}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1128,7 +1128,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{397b421d-0dd2-470c-88b8-f27f976ab327}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a2ea0c6a-ff18-4f72-b284-fe690c2ef476}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1144,7 +1144,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4348135c-e831-4d7e-9f63-b595c8ca2a21}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{66a7bc97-1136-4a90-b7a5-8250f5f0e46e}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1160,7 +1160,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a018f1e1-2581-4132-9edf-2aeb96f4f9c5}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d329bc92-24cd-44df-a3a4-03a40293c811}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1176,7 +1176,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{23e65482-2529-4c63-b813-fa71e94aa499}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{3ff56c14-f048-4303-bd56-f58ed2bf9c15}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1192,7 +1192,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{5410fc0d-2d2a-4667-833f-79053e936acb}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{dc0456df-8719-4666-beac-4ebc197a769a}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1208,7 +1208,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{1caaddde-9f8b-456a-a36e-c30995198589}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{40a3ecb6-a6dc-417a-8ee8-262592a937c6}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1224,7 +1224,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{29bb8ebf-288a-4dc7-9d6a-5885b8779050}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2a0b13e2-cb75-4c4b-9827-7e8f89e3cca0}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1240,7 +1240,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{bc37be61-3cf8-4b96-bd46-8b601da43e37}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{5881b548-c86a-4c01-b3e3-ece26dedee2b}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1256,7 +1256,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{6507d8e1-7579-4ee3-a85e-b4c09a6ac252}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{73be53e9-a4ae-4d16-a453-240b8e56845d}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1272,7 +1272,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{103ac06c-b4fe-414e-a9e5-675122b8ca2e}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b0458139-d1d7-4279-abb3-90f76dc925ed}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1288,7 +1288,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{cd1a2d2e-a65f-4508-8398-9ffa92cf8105}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{453bd5c5-cff4-4e5b-ab09-409848f18093}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1304,7 +1304,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2504a5e7-31fd-494b-bba6-e7137e31a0d6}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{5063bd58-974f-4628-b560-0793ea9f43ed}" type="column" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="0" rightToLeft="0" displayXAxis="1" maxAxisType="Individual" minAxisType="Individual" high="1">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1320,7 +1320,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8199526c-e1e7-43f7-95bb-f6318d400fa2}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c0cc20dc-9707-4200-a186-cf42f7d1a210}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1338,7 +1338,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{66278097-82e0-4f14-981f-6179190897f6}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{d75237fd-ced6-40c4-b3bc-3d3d4cffa425}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1356,7 +1356,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{0d8957bd-4de2-471b-8cf0-ad951fcddf60}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{9409cd51-282f-4396-bda2-da5fd9d861ca}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1374,7 +1374,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a50259dc-ea4b-4eb0-b07f-02233aa8e98b}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{6744498a-d12c-4f42-9966-f3bd0829a878}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1392,7 +1392,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c00865e0-3331-4904-9dd6-84426eabb197}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{67bdee7f-0021-4500-a807-f8dacbec7343}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1410,7 +1410,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{7eebec89-9c7e-41ca-901e-8a32483f8c54}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2c0cd05f-5a67-4b17-8c43-083557b18fa8}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1428,7 +1428,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a3a3d363-f78b-4d07-b7cc-b8e47078eea3}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8584077c-8a2c-460c-a63b-73889455dd9b}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1446,7 +1446,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{82ddfe5e-6d7a-490c-8b43-8cdf9f370ad2}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{9924de4c-7438-4396-b227-2c6e23e9874c}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1464,7 +1464,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{3f2afb21-89d1-429c-b54e-d0b607366a54}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{5a5c174b-63e3-4fd0-88a6-04c815484315}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1482,7 +1482,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8ffa572d-59eb-4bc9-8277-47bcacb5257f}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{1ca7d064-9916-4281-845c-5e7f798c60ff}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1500,7 +1500,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{8cef9304-0307-43f6-a2b5-8855b7bd2c2e}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b88ac959-94aa-466b-8eb4-87f3bea165ee}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1518,7 +1518,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{512e5744-575b-4fab-bdd4-7225a65facd1}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{a7a5521e-49ba-44dd-972f-f737bbb84c96}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1536,7 +1536,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{4b3e4830-7432-4e5e-b92b-afa6492c26d8}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{c689d297-a697-4ca0-9310-b8d2e2dcfb1f}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1554,7 +1554,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{6ae63daf-474b-4fd8-95ba-a2b1f9f25b44}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{12a0407b-b9bc-4496-963b-c7ed1d4f428e}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1572,7 +1572,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{f936dc8c-560a-46e7-b392-07597302fda9}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{767b32c7-18d4-4f6f-8adb-2e02c288f578}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1590,7 +1590,7 @@
           </x14:sparklines>
           <x14:sparklineGroup lineWidth="75"/>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{2dfcc5cc-f843-4be7-93bc-4dd93b13868d}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
+        <x14:sparklineGroup xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:d5p1="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" d5p1:uid="{b1f8ce70-fd5c-4fa8-a8a2-84ff7d759e8c}" type="line" displayHidden="0" displayEmptyCellsAs="zero" dateAxis="1" rightToLeft="0" maxAxisType="Individual" minAxisType="Individual">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>

</xml_diff>